<commit_message>
Update People.xlsx structure with State Name/State Abbreviation column
</commit_message>
<xml_diff>
--- a/DispatcherPrototype/Data/People.xlsx
+++ b/DispatcherPrototype/Data/People.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96aa2c66e503cca3/Documents/UiPath/PrototypeDispatcher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\GitHub\TeamPi-Project2\DispatcherPrototype\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{4C6930E2-B9DE-4DA3-95BE-680B0195167B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C5F5339-821D-4F7A-B241-FD3DC0E3F982}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB69243D-104E-437E-B907-0485B50017EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EFC4AE58-B326-429B-808F-5D674CFBD9D4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EFC4AE58-B326-429B-808F-5D674CFBD9D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -45,9 +45,6 @@
     <t>City</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>angelagongli@gmail.com</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>Wellness</t>
   </si>
   <si>
-    <t>Ill</t>
-  </si>
-  <si>
     <t>Zip Code</t>
   </si>
   <si>
@@ -82,6 +76,18 @@
   </si>
   <si>
     <t>Fort Bend</t>
+  </si>
+  <si>
+    <t>Well</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>State Name</t>
+  </si>
+  <si>
+    <t>State Abbreviation</t>
   </si>
 </sst>
 </file>
@@ -444,23 +450,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56D07A1-5CC8-469C-9D6E-91A50648B6A5}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -469,62 +473,71 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>77063</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>77479</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{27746E09-DD8A-4468-84B3-454BF0CF8FD9}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{1F5554F4-DBE7-4179-83E9-CB3D5E30372D}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{684363AD-AB20-4392-BEBF-F2D810037C0A}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{945BEC65-0752-4C15-87B1-A670C06EF3EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>